<commit_message>
Made modifications to the exercise files according to the notebook and new template format.
</commit_message>
<xml_diff>
--- a/model/data/Exercise/xlsx/StarterTemplate.xlsx
+++ b/model/data/Exercise/xlsx/StarterTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymathradas001\PycharmProjects\pythonProject2\trbs\model\data\Exercise\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A822C892-0542-4415-ACA1-BDA5CBBC814B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294ED322-A225-4B09-AD64-CF45B40A49C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1590" windowWidth="21600" windowHeight="12645" firstSheet="5" activeTab="5" xr2:uid="{4D223BC5-A265-7B41-9F5C-066E948A074C}"/>
+    <workbookView xWindow="-45" yWindow="-18120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="6" xr2:uid="{4D223BC5-A265-7B41-9F5C-066E948A074C}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="90">
   <si>
     <t>configuration</t>
   </si>
@@ -314,9 +314,6 @@
   </si>
   <si>
     <t>% return on clean water investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salary increase per liter of clean water produced </t>
   </si>
 </sst>
 </file>
@@ -451,7 +448,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -475,6 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1082,7 +1080,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C10" sqref="C10:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1322,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1449,6 +1447,7 @@
       <c r="B11" t="s">
         <v>45</v>
       </c>
+      <c r="C11" s="15"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1457,6 +1456,7 @@
       <c r="B12" t="s">
         <v>46</v>
       </c>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1465,6 +1465,7 @@
       <c r="B13" t="s">
         <v>47</v>
       </c>
+      <c r="C13" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1473,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED761DDB-51CF-394F-9D46-C056F7FA6C46}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1666,11 +1667,6 @@
       </c>
       <c r="B23" s="13">
         <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1688,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45498073-CC56-2D41-B5D6-3D03F1233978}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2136,32 +2132,13 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>86</v>
-      </c>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>86</v>
-      </c>
+      <c r="A32" s="14"/>
+      <c r="D32" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
@@ -2180,7 +2157,7 @@
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:D32">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2190,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E05F8AE-8DA8-724A-AD7F-0A10B8E741F3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2233,6 +2210,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2291,10 +2269,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A5">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A5">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>